<commit_message>
[.xlsx] grouped the data from my my investigation
</commit_message>
<xml_diff>
--- a/manual/ja/ja_Investigation_results.xlsx
+++ b/manual/ja/ja_Investigation_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Downloads/Investigation_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B256EB-B352-1244-9567-7D703BF3171D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F3D614-A975-462D-AE72-1034944B9A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munkalap1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>IP address</t>
   </si>
@@ -73,71 +73,125 @@
     <t>Other information</t>
   </si>
   <si>
-    <t>99.99.99.99</t>
-  </si>
-  <si>
-    <t>99.99.99.0/24</t>
-  </si>
-  <si>
-    <t>Example A/S</t>
-  </si>
-  <si>
-    <t>ISP sample A/S</t>
-  </si>
-  <si>
-    <t>Commercial</t>
-  </si>
-  <si>
     <t>Copenhagen</t>
   </si>
   <si>
-    <t>malicious_block1</t>
-  </si>
-  <si>
-    <t>virustotal: -34, abuseipdb: 34%</t>
-  </si>
-  <si>
-    <t>SSH bruteforce</t>
-  </si>
-  <si>
-    <t>22 SSH</t>
-  </si>
-  <si>
-    <t>examp.dk</t>
-  </si>
-  <si>
-    <t>HTTP response 301</t>
-  </si>
-  <si>
-    <t>2 files: malicious, trojan</t>
-  </si>
-  <si>
-    <t>Zxy router</t>
-  </si>
-  <si>
-    <t>Probably</t>
-  </si>
-  <si>
-    <t>Mirai botnet</t>
-  </si>
-  <si>
     <t>Used websites, tools</t>
   </si>
   <si>
-    <t>virustotal, abuseipdb, greynoise</t>
-  </si>
-  <si>
     <t>Please upload your findings to this table. There is an example row (yellow background). Use different background colour please.</t>
+  </si>
+  <si>
+    <t>130.225.39.160</t>
+  </si>
+  <si>
+    <t>130.225.0.0/16</t>
+  </si>
+  <si>
+    <t> FSKNET-DK Forskningsnettet - Danish network for Research and Education</t>
+  </si>
+  <si>
+    <t>Research and Education</t>
+  </si>
+  <si>
+    <t>DRONE BL</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>22 SSH / TCP</t>
+  </si>
+  <si>
+    <t>Different encryption methods</t>
+  </si>
+  <si>
+    <t>aau-cloud maybe?</t>
+  </si>
+  <si>
+    <t>Aalborg Universitet, DTU, DeiC Netdrift</t>
+  </si>
+  <si>
+    <t>Probably not</t>
+  </si>
+  <si>
+    <t>virustotal, abuseipdb, shodan</t>
+  </si>
+  <si>
+    <t>130.225.244.90</t>
+  </si>
+  <si>
+    <t>DTU</t>
+  </si>
+  <si>
+    <t>virustotal: 0, abuseipdb: N/A</t>
+  </si>
+  <si>
+    <t>virustotal: -1, abuseipdb: 0%</t>
+  </si>
+  <si>
+    <t>dotsrc.org</t>
+  </si>
+  <si>
+    <t>DAN TOR, s5h.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C&amp;C botnet, </t>
+  </si>
+  <si>
+    <t>Tor-node</t>
+  </si>
+  <si>
+    <t>80/TCP, 161/UDP, 9001/TCP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">botnet, bruteforce, ssh, port scan </t>
+  </si>
+  <si>
+    <t>SSL certificate, net-snmp, HTTP/1.0 404 Not found</t>
+  </si>
+  <si>
+    <t>80.209.87.103</t>
+  </si>
+  <si>
+    <t>Fibia</t>
+  </si>
+  <si>
+    <t>Peer2Peer electronic cash system</t>
+  </si>
+  <si>
+    <t>Hornsyld</t>
+  </si>
+  <si>
+    <t>Miner</t>
+  </si>
+  <si>
+    <t>https://www.electroncash.dk/bitcoin.pdf, https://3.dk.pool.ntp.org/?lang=zh, electroncash.dk</t>
+  </si>
+  <si>
+    <t>SSL certificate,  220 I'm as free as a bird now</t>
+  </si>
+  <si>
+    <t>80/TCP, 123/UDP, 443/TCP, 60001/TCP, 60010/TCP</t>
+  </si>
+  <si>
+    <t>Some different malicious</t>
+  </si>
+  <si>
+    <t>80.209.0.0/17</t>
+  </si>
+  <si>
+    <t>oninoin site linked on the clear web page, PDF to the bitcoin paper</t>
+  </si>
+  <si>
+    <t>Unknown private person probably</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -161,13 +215,32 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,18 +255,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE599"/>
-        <bgColor rgb="FFFFE599"/>
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor rgb="FFEFEFEF"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -216,20 +293,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bemærk!" xfId="2" builtinId="10"/>
+    <cellStyle name="God" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,71 +545,73 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A3:R6"/>
+  <dimension ref="A3:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="5" width="12.5" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
-    <col min="8" max="8" width="35.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" customWidth="1"/>
-    <col min="14" max="14" width="20.5" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="60.5703125" customWidth="1"/>
+    <col min="4" max="4" width="105.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" customWidth="1"/>
+    <col min="9" max="9" width="32" customWidth="1"/>
+    <col min="10" max="10" width="87.85546875" customWidth="1"/>
+    <col min="11" max="11" width="95.42578125" customWidth="1"/>
+    <col min="12" max="12" width="47" customWidth="1"/>
+    <col min="13" max="13" width="30" customWidth="1"/>
+    <col min="14" max="14" width="29.85546875" customWidth="1"/>
+    <col min="15" max="15" width="26.5703125" customWidth="1"/>
     <col min="16" max="16" width="49" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" customWidth="1"/>
-    <col min="18" max="18" width="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="81.28515625" customWidth="1"/>
+    <col min="18" max="18" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,64 +663,176 @@
       <c r="Q5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="9">
+        <v>44980</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="7">
+        <v>42130</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" s="3">
-        <v>44927</v>
-      </c>
-      <c r="P6" s="2" t="s">
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="R8" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -627,5 +840,6 @@
     <mergeCell ref="A3:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>